<commit_message>
added stagingSystem to staging csv; supported through template process
</commit_message>
<xml_diff>
--- a/docs/CSV Templates 20200806.xlsx
+++ b/docs/CSV Templates 20200806.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacarter/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dphelan/Development/mcode-extraction-framework/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B57A7C0-A6AB-0C42-835F-91E1BAB6B3DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7DBA28-90EE-174D-B6DE-649F34ABD872}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="6" xr2:uid="{1BB3AE08-1F40-234D-9B08-AA5ABD9D5659}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="5" xr2:uid="{1BB3AE08-1F40-234D-9B08-AA5ABD9D5659}"/>
   </bookViews>
   <sheets>
     <sheet name="CancerPatient" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="133">
   <si>
     <t>conditionId</t>
   </si>
@@ -755,6 +755,12 @@
   </si>
   <si>
     <t>The state of the medication used that this statement is about. Generally will be active or completed.</t>
+  </si>
+  <si>
+    <t>stagingSystem</t>
+  </si>
+  <si>
+    <t>System used for staging, chosen from the mCODE valueset: http://hl7.org/fhir/us/mcode/ValueSet-mcode-cancer-staging-system-vs.html</t>
   </si>
 </sst>
 </file>
@@ -880,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -932,6 +938,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1982,10 +1991,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6DE738-FA5B-814A-88BE-E5AE170BABF4}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1997,11 +2006,12 @@
     <col min="5" max="5" width="18.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" style="5" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="5"/>
+    <col min="8" max="8" width="47.83203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -2024,10 +2034,13 @@
         <v>42</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>57</v>
       </c>
@@ -2049,11 +2062,14 @@
       <c r="G2" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>121</v>
       </c>
@@ -2064,22 +2080,22 @@
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
     </row>
-    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -2096,7 +2112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966793A4-4CC8-2E4D-BE70-7ABF76162552}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
@@ -2236,18 +2252,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2448,18 +2464,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C39A211E-8FA7-4907-9A49-0A4E41B12870}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32E0DDC2-8F58-4E50-9FE3-C75BD101647B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32E0DDC2-8F58-4E50-9FE3-C75BD101647B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C39A211E-8FA7-4907-9A49-0A4E41B12870}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>